<commit_message>
Standard Base Parameter für die Trainings
</commit_message>
<xml_diff>
--- a/gym_pybullet_drones/examples/maze_urdf_test/self_made_maps/maps/map_24_INIT_Positions.xlsx
+++ b/gym_pybullet_drones/examples/maze_urdf_test/self_made_maps/maps/map_24_INIT_Positions.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">Index 1</t>
+    <t xml:space="preserve">Index 2</t>
   </si>
   <si>
     <t xml:space="preserve">Startpunkte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index 1</t>
   </si>
   <si>
     <t xml:space="preserve">Index 2 </t>
@@ -254,10 +260,10 @@
   <dimension ref="A1:BR62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BQ3" activeCellId="0" sqref="BQ3:BR12"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="2" style="0" width="2.54"/>
@@ -461,16 +467,16 @@
         <v>2</v>
       </c>
       <c r="BO2" s="0" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BP2" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BQ2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BR2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Training auf schwerren Mazes abgeschlossen, besser als vorher, aber nicht ganz idael. Evtl.Probleme mit der Qualität der Slammap bzw. Mazes zu eng?!
</commit_message>
<xml_diff>
--- a/gym_pybullet_drones/examples/maze_urdf_test/self_made_maps/maps/map_24_INIT_Positions.xlsx
+++ b/gym_pybullet_drones/examples/maze_urdf_test/self_made_maps/maps/map_24_INIT_Positions.xlsx
@@ -20,18 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Index 2</t>
+    <t xml:space="preserve">Index 1</t>
   </si>
   <si>
     <t xml:space="preserve">Startpunkte</t>
   </si>
   <si>
-    <t xml:space="preserve">Index 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index 1</t>
+    <t xml:space="preserve">Index 2</t>
   </si>
   <si>
     <t xml:space="preserve">Index 2 </t>
@@ -259,11 +256,11 @@
   </sheetPr>
   <dimension ref="A1:BR62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AY1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BQ14" activeCellId="0" sqref="BQ14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="2" style="0" width="2.54"/>
@@ -276,184 +273,184 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
         <v>59</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="AD1" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="AE1" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="AF1" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AI1" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AJ1" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AL1" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="AM1" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="AN1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="AO1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="AP1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="AQ1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="AR1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="AS1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="AT1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="AU1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="AV1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="AW1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="AX1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="AY1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="AZ1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="BA1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="BB1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="BC1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="BD1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="BE1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BF1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="BG1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="BH1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="BI1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ1" s="1" t="n">
-        <v>0</v>
       </c>
       <c r="BK1" s="2" t="s">
         <v>0</v>
@@ -467,16 +464,16 @@
         <v>2</v>
       </c>
       <c r="BO2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BP2" s="3" t="s">
+      <c r="BQ2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="BQ2" s="0" t="s">
+      <c r="BR2" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="BR2" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,14 +664,14 @@
         <v>1</v>
       </c>
       <c r="BO3" s="0" t="n">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="BP3" s="0" t="n">
         <v>9</v>
       </c>
       <c r="BQ3" s="0" t="n">
         <f aca="false">BO3*0.05</f>
-        <v>0.55</v>
+        <v>2.4</v>
       </c>
       <c r="BR3" s="0" t="n">
         <f aca="false">BP3*0.05</f>
@@ -695,14 +692,14 @@
         <v>2</v>
       </c>
       <c r="BO4" s="0" t="n">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="BP4" s="0" t="n">
         <v>25</v>
       </c>
       <c r="BQ4" s="0" t="n">
         <f aca="false">BO4*0.05</f>
-        <v>0.8</v>
+        <v>2.15</v>
       </c>
       <c r="BR4" s="0" t="n">
         <f aca="false">BP4*0.05</f>
@@ -723,14 +720,14 @@
         <v>3</v>
       </c>
       <c r="BO5" s="0" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="BP5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="BQ5" s="0" t="n">
         <f aca="false">BO5*0.05</f>
-        <v>1.8</v>
+        <v>1.15</v>
       </c>
       <c r="BR5" s="0" t="n">
         <f aca="false">BP5*0.05</f>
@@ -751,14 +748,14 @@
         <v>4</v>
       </c>
       <c r="BO6" s="0" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="BP6" s="0" t="n">
         <v>15</v>
       </c>
       <c r="BQ6" s="0" t="n">
         <f aca="false">BO6*0.05</f>
-        <v>2.5</v>
+        <v>0.45</v>
       </c>
       <c r="BR6" s="0" t="n">
         <f aca="false">BP6*0.05</f>
@@ -780,14 +777,14 @@
         <v>5</v>
       </c>
       <c r="BO7" s="0" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="BP7" s="0" t="n">
         <v>26</v>
       </c>
       <c r="BQ7" s="0" t="n">
         <f aca="false">BO7*0.05</f>
-        <v>1.75</v>
+        <v>1.2</v>
       </c>
       <c r="BR7" s="0" t="n">
         <f aca="false">BP7*0.05</f>
@@ -808,14 +805,14 @@
         <v>6</v>
       </c>
       <c r="BO8" s="0" t="n">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="BP8" s="0" t="n">
         <v>38</v>
       </c>
       <c r="BQ8" s="0" t="n">
         <f aca="false">BO8*0.05</f>
-        <v>1.9</v>
+        <v>1.05</v>
       </c>
       <c r="BR8" s="0" t="n">
         <f aca="false">BP8*0.05</f>
@@ -839,14 +836,14 @@
         <v>7</v>
       </c>
       <c r="BO9" s="0" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="BP9" s="0" t="n">
         <v>43</v>
       </c>
       <c r="BQ9" s="0" t="n">
         <f aca="false">BO9*0.05</f>
-        <v>2.65</v>
+        <v>0.3</v>
       </c>
       <c r="BR9" s="0" t="n">
         <f aca="false">BP9*0.05</f>
@@ -867,14 +864,14 @@
         <v>8</v>
       </c>
       <c r="BO10" s="0" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="BP10" s="0" t="n">
         <v>47</v>
       </c>
       <c r="BQ10" s="0" t="n">
         <f aca="false">BO10*0.05</f>
-        <v>1.65</v>
+        <v>1.3</v>
       </c>
       <c r="BR10" s="0" t="n">
         <f aca="false">BP10*0.05</f>
@@ -895,14 +892,14 @@
         <v>9</v>
       </c>
       <c r="BO11" s="0" t="n">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="BP11" s="0" t="n">
         <v>52</v>
       </c>
       <c r="BQ11" s="0" t="n">
         <f aca="false">BO11*0.05</f>
-        <v>0.9</v>
+        <v>2.05</v>
       </c>
       <c r="BR11" s="0" t="n">
         <f aca="false">BP11*0.05</f>
@@ -926,14 +923,14 @@
         <v>10</v>
       </c>
       <c r="BO12" s="0" t="n">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="BP12" s="0" t="n">
         <v>45</v>
       </c>
       <c r="BQ12" s="0" t="n">
         <f aca="false">BO12*0.05</f>
-        <v>0.55</v>
+        <v>2.4</v>
       </c>
       <c r="BR12" s="0" t="n">
         <f aca="false">BP12*0.05</f>

</xml_diff>